<commit_message>
preparation for SCCS release based on WP4 SCCS sensitivity code for publication in development
</commit_message>
<xml_diff>
--- a/p_parameters/archive_parameters/Variables_ALG_DP_ROC20_20Apr23.xlsx
+++ b/p_parameters/archive_parameters/Variables_ALG_DP_ROC20_20Apr23.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\CVM_development_1811\p_parameters\archive_parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cduransa/Documents/Utrecht/ROC20/WP3/CVM/Script development/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F776784-BE2D-4A46-9C8C-F743364ACBE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{3C1EF13E-4883-5043-98F8-7ECB9CA3F8DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D87366D5-C98D-483E-B8A5-5C1A9A36C0CB}"/>
   <bookViews>
-    <workbookView xWindow="585" yWindow="1005" windowWidth="14760" windowHeight="15900" xr2:uid="{2506CD93-0285-9E44-BBDD-A2C4E77A0341}"/>
+    <workbookView xWindow="580" yWindow="1000" windowWidth="14760" windowHeight="15900" xr2:uid="{2506CD93-0285-9E44-BBDD-A2C4E77A0341}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,7 @@
     <sheet name="DrugProxies" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ALG!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$G$127</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$F$104</definedName>
   </definedNames>
   <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
@@ -31,10 +30,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="184">
   <si>
     <t>Varname</t>
   </si>
@@ -635,7 +634,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -690,20 +689,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -731,7 +729,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1046,20 +1044,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D760FD20-DA31-7D44-AA6E-1B0770159217}">
-  <dimension ref="A1:G127"/>
+  <dimension ref="A1:G128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="35.625" customWidth="1"/>
     <col min="6" max="6" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1082,7 +1080,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1105,7 +1103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1128,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1151,12 +1149,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -1174,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1197,7 +1195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1220,7 +1218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1243,12 +1241,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -1266,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1289,7 +1287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1312,7 +1310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1335,7 +1333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1358,7 +1356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1381,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1404,7 +1402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1427,7 +1425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1450,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1473,7 +1471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1496,7 +1494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1519,7 +1517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1542,7 +1540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1565,7 +1563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1588,7 +1586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1611,7 +1609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1634,7 +1632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1657,7 +1655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1680,7 +1678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1703,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1726,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1749,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1772,7 +1770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1795,7 +1793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -1818,7 +1816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1841,7 +1839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -1864,7 +1862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -1887,7 +1885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1910,7 +1908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -1933,7 +1931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -1956,7 +1954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -1979,7 +1977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -2002,7 +2000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -2025,7 +2023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -2048,7 +2046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -2071,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -2094,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -2117,7 +2115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -2140,7 +2138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -2163,7 +2161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -2186,7 +2184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -2209,7 +2207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -2232,7 +2230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>57</v>
       </c>
@@ -2255,7 +2253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -2278,7 +2276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>59</v>
       </c>
@@ -2301,7 +2299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -2324,7 +2322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -2347,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>62</v>
       </c>
@@ -2370,7 +2368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -2393,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>64</v>
       </c>
@@ -2416,7 +2414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>65</v>
       </c>
@@ -2439,7 +2437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -2462,7 +2460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7">
       <c r="A62" t="s">
         <v>67</v>
       </c>
@@ -2485,7 +2483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -2508,7 +2506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -2531,7 +2529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>69</v>
       </c>
@@ -2554,7 +2552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -2577,7 +2575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>71</v>
       </c>
@@ -2600,7 +2598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>72</v>
       </c>
@@ -2623,7 +2621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>73</v>
       </c>
@@ -2646,7 +2644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>74</v>
       </c>
@@ -2669,7 +2667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>75</v>
       </c>
@@ -2692,7 +2690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>76</v>
       </c>
@@ -2715,7 +2713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>77</v>
       </c>
@@ -2738,7 +2736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
         <v>78</v>
       </c>
@@ -2761,7 +2759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7">
       <c r="A75" t="s">
         <v>79</v>
       </c>
@@ -2784,7 +2782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7">
       <c r="A76" t="s">
         <v>80</v>
       </c>
@@ -2807,7 +2805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
         <v>81</v>
       </c>
@@ -2830,7 +2828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
         <v>82</v>
       </c>
@@ -2853,7 +2851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7">
       <c r="A79" t="s">
         <v>83</v>
       </c>
@@ -2876,7 +2874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7">
       <c r="A80" t="s">
         <v>84</v>
       </c>
@@ -2899,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
         <v>85</v>
       </c>
@@ -2922,7 +2920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7">
       <c r="A82" t="s">
         <v>86</v>
       </c>
@@ -2945,7 +2943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7">
       <c r="A83" t="s">
         <v>87</v>
       </c>
@@ -2968,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7">
       <c r="A84" t="s">
         <v>88</v>
       </c>
@@ -2991,7 +2989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
         <v>89</v>
       </c>
@@ -3014,7 +3012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7">
       <c r="A86" t="s">
         <v>90</v>
       </c>
@@ -3037,7 +3035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7">
       <c r="A87" t="s">
         <v>91</v>
       </c>
@@ -3060,7 +3058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7">
       <c r="A88" t="s">
         <v>92</v>
       </c>
@@ -3083,7 +3081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
         <v>93</v>
       </c>
@@ -3106,7 +3104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7">
       <c r="A90" t="s">
         <v>94</v>
       </c>
@@ -3129,7 +3127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7">
       <c r="A91" t="s">
         <v>95</v>
       </c>
@@ -3152,7 +3150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7">
       <c r="A92" t="s">
         <v>96</v>
       </c>
@@ -3175,7 +3173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7">
       <c r="A93" t="s">
         <v>97</v>
       </c>
@@ -3198,7 +3196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7">
       <c r="A94" t="s">
         <v>98</v>
       </c>
@@ -3221,7 +3219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7">
       <c r="A95" t="s">
         <v>99</v>
       </c>
@@ -3244,7 +3242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7">
       <c r="A96" t="s">
         <v>100</v>
       </c>
@@ -3267,7 +3265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7">
       <c r="A97" t="s">
         <v>101</v>
       </c>
@@ -3290,7 +3288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7">
       <c r="A98" t="s">
         <v>102</v>
       </c>
@@ -3313,7 +3311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7">
       <c r="A99" t="s">
         <v>103</v>
       </c>
@@ -3336,7 +3334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7">
       <c r="A100" t="s">
         <v>104</v>
       </c>
@@ -3359,7 +3357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7">
       <c r="A101" t="s">
         <v>105</v>
       </c>
@@ -3382,7 +3380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7">
       <c r="A102" t="s">
         <v>106</v>
       </c>
@@ -3405,7 +3403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7">
       <c r="A103" s="6" t="s">
         <v>107</v>
       </c>
@@ -3428,7 +3426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7">
       <c r="A104" s="6" t="s">
         <v>108</v>
       </c>
@@ -3451,7 +3449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7">
       <c r="A105" t="s">
         <v>109</v>
       </c>
@@ -3474,7 +3472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7">
       <c r="A106" s="6" t="s">
         <v>110</v>
       </c>
@@ -3497,7 +3495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7">
       <c r="A107" s="6" t="s">
         <v>111</v>
       </c>
@@ -3520,7 +3518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7">
       <c r="A108" s="6" t="s">
         <v>112</v>
       </c>
@@ -3543,7 +3541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7">
       <c r="A109" s="6" t="s">
         <v>113</v>
       </c>
@@ -3566,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7">
       <c r="A110" t="s">
         <v>114</v>
       </c>
@@ -3589,7 +3587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7">
       <c r="A111" t="s">
         <v>115</v>
       </c>
@@ -3612,7 +3610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7">
       <c r="A112" t="s">
         <v>116</v>
       </c>
@@ -3635,7 +3633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7">
       <c r="A113" t="s">
         <v>117</v>
       </c>
@@ -3658,7 +3656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7">
       <c r="A114" t="s">
         <v>118</v>
       </c>
@@ -3681,7 +3679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7">
       <c r="A115" t="s">
         <v>119</v>
       </c>
@@ -3704,7 +3702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7">
       <c r="A116" t="s">
         <v>120</v>
       </c>
@@ -3727,7 +3725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7">
       <c r="A117" t="s">
         <v>121</v>
       </c>
@@ -3750,7 +3748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7">
       <c r="A118" t="s">
         <v>122</v>
       </c>
@@ -3773,7 +3771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7">
       <c r="A119" t="s">
         <v>123</v>
       </c>
@@ -3796,7 +3794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7">
       <c r="A120" t="s">
         <v>124</v>
       </c>
@@ -3819,7 +3817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7">
       <c r="A121" t="s">
         <v>125</v>
       </c>
@@ -3842,7 +3840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7">
       <c r="A122" t="s">
         <v>126</v>
       </c>
@@ -3865,7 +3863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7">
       <c r="A123" t="s">
         <v>127</v>
       </c>
@@ -3888,7 +3886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7">
       <c r="A124" t="s">
         <v>128</v>
       </c>
@@ -3911,7 +3909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7">
       <c r="A125" t="s">
         <v>129</v>
       </c>
@@ -3934,7 +3932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7">
       <c r="A126" t="s">
         <v>130</v>
       </c>
@@ -3957,7 +3955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7">
       <c r="A127" t="s">
         <v>125</v>
       </c>
@@ -3980,28 +3978,55 @@
         <v>1</v>
       </c>
     </row>
+    <row r="128" spans="1:7">
+      <c r="A128" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B128" t="b">
+        <v>1</v>
+      </c>
+      <c r="C128" t="b">
+        <v>0</v>
+      </c>
+      <c r="D128" t="b">
+        <v>0</v>
+      </c>
+      <c r="E128" t="b">
+        <v>0</v>
+      </c>
+      <c r="F128" t="b">
+        <v>0</v>
+      </c>
+      <c r="G128" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G127" xr:uid="{D760FD20-DA31-7D44-AA6E-1B0770159217}"/>
+  <autoFilter ref="A1:F127" xr:uid="{D760FD20-DA31-7D44-AA6E-1B0770159217}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F104">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D84700-DED7-384E-8400-81ED0D9F0B97}">
-  <dimension ref="A1:J80"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="3" max="3" width="35.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.5" customWidth="1"/>
     <col min="5" max="5" width="25.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>131</v>
       </c>
@@ -4033,7 +4058,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -4062,7 +4087,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>140</v>
       </c>
@@ -4091,7 +4116,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -4120,7 +4145,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>140</v>
       </c>
@@ -4149,7 +4174,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -4178,7 +4203,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>140</v>
       </c>
@@ -4207,7 +4232,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>140</v>
       </c>
@@ -4236,7 +4261,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>140</v>
       </c>
@@ -4265,7 +4290,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>140</v>
       </c>
@@ -4294,7 +4319,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>140</v>
       </c>
@@ -4323,7 +4348,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -4352,7 +4377,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -4381,7 +4406,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>140</v>
       </c>
@@ -4410,7 +4435,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>140</v>
       </c>
@@ -4439,7 +4464,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -4468,7 +4493,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>140</v>
       </c>
@@ -4497,7 +4522,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -4526,7 +4551,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>140</v>
       </c>
@@ -4555,7 +4580,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>140</v>
       </c>
@@ -4584,7 +4609,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>140</v>
       </c>
@@ -4613,7 +4638,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>140</v>
       </c>
@@ -4642,7 +4667,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>140</v>
       </c>
@@ -4671,7 +4696,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>140</v>
       </c>
@@ -4700,7 +4725,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>140</v>
       </c>
@@ -4729,7 +4754,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>140</v>
       </c>
@@ -4758,7 +4783,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>140</v>
       </c>
@@ -4787,7 +4812,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -4816,7 +4841,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>140</v>
       </c>
@@ -4845,7 +4870,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>140</v>
       </c>
@@ -4874,7 +4899,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>140</v>
       </c>
@@ -4903,7 +4928,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>140</v>
       </c>
@@ -4932,7 +4957,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>140</v>
       </c>
@@ -4961,7 +4986,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>140</v>
       </c>
@@ -4990,7 +5015,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>140</v>
       </c>
@@ -5019,7 +5044,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>140</v>
       </c>
@@ -5048,7 +5073,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>140</v>
       </c>
@@ -5077,7 +5102,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>140</v>
       </c>
@@ -5106,7 +5131,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>140</v>
       </c>
@@ -5135,7 +5160,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>140</v>
       </c>
@@ -5164,7 +5189,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>140</v>
       </c>
@@ -5193,7 +5218,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>140</v>
       </c>
@@ -5222,7 +5247,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>140</v>
       </c>
@@ -5251,7 +5276,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
         <v>140</v>
       </c>
@@ -5280,7 +5305,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
         <v>140</v>
       </c>
@@ -5309,7 +5334,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
         <v>140</v>
       </c>
@@ -5338,7 +5363,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
         <v>140</v>
       </c>
@@ -5367,7 +5392,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
         <v>140</v>
       </c>
@@ -5396,7 +5421,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>140</v>
       </c>
@@ -5425,7 +5450,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>140</v>
       </c>
@@ -5454,7 +5479,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>140</v>
       </c>
@@ -5483,7 +5508,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
         <v>140</v>
       </c>
@@ -5512,7 +5537,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" t="s">
         <v>140</v>
       </c>
@@ -5541,7 +5566,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" t="s">
         <v>140</v>
       </c>
@@ -5570,7 +5595,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" t="s">
         <v>140</v>
       </c>
@@ -5599,7 +5624,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" t="s">
         <v>140</v>
       </c>
@@ -5628,7 +5653,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" t="s">
         <v>140</v>
       </c>
@@ -5657,7 +5682,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" t="s">
         <v>140</v>
       </c>
@@ -5686,7 +5711,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" t="s">
         <v>140</v>
       </c>
@@ -5715,7 +5740,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" t="s">
         <v>140</v>
       </c>
@@ -5744,7 +5769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" t="s">
         <v>140</v>
       </c>
@@ -5754,7 +5779,7 @@
       <c r="C61" t="s">
         <v>15</v>
       </c>
-      <c r="D61" s="8" t="s">
+      <c r="D61" s="6" t="s">
         <v>107</v>
       </c>
       <c r="F61">
@@ -5773,7 +5798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" t="s">
         <v>140</v>
       </c>
@@ -5783,7 +5808,7 @@
       <c r="C62" t="s">
         <v>15</v>
       </c>
-      <c r="D62" s="8" t="s">
+      <c r="D62" t="s">
         <v>91</v>
       </c>
       <c r="F62">
@@ -5802,7 +5827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" t="s">
         <v>140</v>
       </c>
@@ -5812,7 +5837,7 @@
       <c r="C63" t="s">
         <v>15</v>
       </c>
-      <c r="D63" s="8" t="s">
+      <c r="D63" t="s">
         <v>16</v>
       </c>
       <c r="F63">
@@ -5831,7 +5856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" t="s">
         <v>140</v>
       </c>
@@ -5841,7 +5866,7 @@
       <c r="C64" t="s">
         <v>15</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="D64" t="s">
         <v>74</v>
       </c>
       <c r="F64">
@@ -5860,7 +5885,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
         <v>140</v>
       </c>
@@ -5870,7 +5895,7 @@
       <c r="C65" t="s">
         <v>15</v>
       </c>
-      <c r="D65" s="8" t="s">
+      <c r="D65" t="s">
         <v>14</v>
       </c>
       <c r="F65">
@@ -5889,7 +5914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" t="s">
         <v>140</v>
       </c>
@@ -5899,11 +5924,11 @@
       <c r="C66" t="s">
         <v>15</v>
       </c>
-      <c r="D66" s="8" t="s">
+      <c r="D66" s="6" t="s">
         <v>109</v>
       </c>
       <c r="F66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G66" t="s">
         <v>141</v>
@@ -5918,7 +5943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
         <v>140</v>
       </c>
@@ -5926,28 +5951,28 @@
         <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>15</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>104</v>
+        <v>7</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>107</v>
       </c>
       <c r="F67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G67" t="s">
         <v>141</v>
       </c>
       <c r="H67" t="s">
-        <v>145</v>
-      </c>
-      <c r="I67">
-        <v>-10</v>
-      </c>
-      <c r="J67">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="I67" t="s">
+        <v>142</v>
+      </c>
+      <c r="J67" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68" t="s">
         <v>140</v>
       </c>
@@ -5957,8 +5982,8 @@
       <c r="C68" t="s">
         <v>7</v>
       </c>
-      <c r="D68" s="8" t="s">
-        <v>107</v>
+      <c r="D68" t="s">
+        <v>82</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -5976,7 +6001,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
         <v>140</v>
       </c>
@@ -5987,7 +6012,7 @@
         <v>7</v>
       </c>
       <c r="D69" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -6005,7 +6030,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
         <v>140</v>
       </c>
@@ -6016,7 +6041,7 @@
         <v>7</v>
       </c>
       <c r="D70" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -6034,7 +6059,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" t="s">
         <v>140</v>
       </c>
@@ -6045,7 +6070,7 @@
         <v>7</v>
       </c>
       <c r="D71" t="s">
-        <v>81</v>
+        <v>8</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -6063,7 +6088,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -6074,7 +6099,7 @@
         <v>7</v>
       </c>
       <c r="D72" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -6092,7 +6117,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
         <v>140</v>
       </c>
@@ -6103,7 +6128,7 @@
         <v>7</v>
       </c>
       <c r="D73" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F73">
         <v>1</v>
@@ -6121,7 +6146,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" t="s">
         <v>140</v>
       </c>
@@ -6132,7 +6157,7 @@
         <v>7</v>
       </c>
       <c r="D74" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -6150,7 +6175,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" t="s">
         <v>140</v>
       </c>
@@ -6160,26 +6185,11 @@
       <c r="C75" t="s">
         <v>7</v>
       </c>
-      <c r="D75" t="s">
-        <v>13</v>
-      </c>
-      <c r="F75">
-        <v>1</v>
-      </c>
-      <c r="G75" t="s">
-        <v>141</v>
-      </c>
-      <c r="H75" t="s">
-        <v>142</v>
-      </c>
-      <c r="I75" t="s">
-        <v>142</v>
-      </c>
-      <c r="J75" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D75" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
         <v>140</v>
       </c>
@@ -6190,24 +6200,39 @@
         <v>7</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
         <v>140</v>
       </c>
       <c r="B77" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C77" t="s">
-        <v>7</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="D77" t="s">
+        <v>47</v>
+      </c>
+      <c r="F77">
+        <v>1</v>
+      </c>
+      <c r="G77" t="s">
+        <v>141</v>
+      </c>
+      <c r="H77" t="s">
+        <v>142</v>
+      </c>
+      <c r="I77" t="s">
+        <v>142</v>
+      </c>
+      <c r="J77" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
         <v>140</v>
       </c>
@@ -6218,7 +6243,7 @@
         <v>48</v>
       </c>
       <c r="D78" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="F78">
         <v>1</v>
@@ -6236,7 +6261,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
         <v>140</v>
       </c>
@@ -6246,8 +6271,8 @@
       <c r="C79" t="s">
         <v>48</v>
       </c>
-      <c r="D79" t="s">
-        <v>99</v>
+      <c r="D79" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="F79">
         <v>1</v>
@@ -6265,37 +6290,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>140</v>
-      </c>
-      <c r="B80" t="s">
-        <v>2</v>
-      </c>
-      <c r="C80" t="s">
-        <v>48</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="F80">
-        <v>1</v>
-      </c>
-      <c r="G80" t="s">
-        <v>141</v>
-      </c>
-      <c r="H80" t="s">
-        <v>142</v>
-      </c>
-      <c r="I80" t="s">
-        <v>142</v>
-      </c>
-      <c r="J80" t="s">
-        <v>142</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:J80" xr:uid="{69D84700-DED7-384E-8400-81ED0D9F0B97}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6308,7 +6303,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="1" max="1" width="25.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.625" bestFit="1" customWidth="1"/>
@@ -6316,7 +6311,7 @@
     <col min="4" max="4" width="35.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>146</v>
       </c>
@@ -6330,7 +6325,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -6341,7 +6336,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -6352,7 +6347,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -6363,7 +6358,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -6377,7 +6372,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -6391,7 +6386,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -6405,7 +6400,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -6419,7 +6414,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -6433,7 +6428,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -6447,7 +6442,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -6461,7 +6456,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -6475,7 +6470,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -6489,7 +6484,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -6503,7 +6498,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -6514,7 +6509,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -6525,7 +6520,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -6536,7 +6531,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -6547,7 +6542,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>125</v>
       </c>
@@ -6567,6 +6562,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6dac44d48b4406d5c320fe911a853389">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="183e839aabd2ef2c305af4a754f6d8de" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -6811,15 +6815,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6833,39 +6828,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48B15A9D-CB22-48CA-A07F-E7C6B66686BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89B141F6-1B65-48D6-AC6D-6863CE810BB1}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89B141F6-1B65-48D6-AC6D-6863CE810BB1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48B15A9D-CB22-48CA-A07F-E7C6B66686BD}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{794DD23A-82BD-4D35-84D2-4A4CA4219C4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{794DD23A-82BD-4D35-84D2-4A4CA4219C4A}"/>
 </file>
</xml_diff>